<commit_message>
Updated to include pcb, sensor and wireless variants
</commit_message>
<xml_diff>
--- a/GDBP/Device Permutations/components.xlsx
+++ b/GDBP/Device Permutations/components.xlsx
@@ -1,104 +1,220 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09112E4-DCF2-4EE6-B0D8-472E0F698DF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\Programming\Uni\trunk\GDBP\Device Permutations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1931ECB-6821-4C3A-9A96-FA626687C2FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <si>
+    <t>Component Name</t>
+  </si>
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Component Name</t>
-  </si>
-  <si>
-    <t>Unit Price</t>
-  </si>
-  <si>
-    <t>Unit Volume</t>
-  </si>
-  <si>
-    <t>Quantity Needed (per Device)</t>
-  </si>
-  <si>
-    <t>Sensor 1</t>
-  </si>
-  <si>
-    <t>Sensor 2</t>
-  </si>
-  <si>
-    <t>Sensor 3</t>
-  </si>
-  <si>
-    <t>Wireless 1</t>
-  </si>
-  <si>
-    <t>Wireless 2</t>
-  </si>
-  <si>
-    <t>Wireless 3</t>
-  </si>
-  <si>
-    <t>Battery 1</t>
-  </si>
-  <si>
-    <t>Battery 2</t>
-  </si>
-  <si>
-    <t>Battery 3</t>
-  </si>
-  <si>
-    <t>S001</t>
-  </si>
-  <si>
-    <t>S002</t>
-  </si>
-  <si>
-    <t>S003</t>
-  </si>
-  <si>
-    <t>W001</t>
-  </si>
-  <si>
-    <t>W002</t>
-  </si>
-  <si>
-    <t>W003</t>
-  </si>
-  <si>
-    <t>B001</t>
-  </si>
-  <si>
-    <t>B002</t>
-  </si>
-  <si>
-    <t>B003</t>
+    <t>Unit Price at 5000 batch (£)</t>
+  </si>
+  <si>
+    <t>Unit Volume (mm3)</t>
+  </si>
+  <si>
+    <t>Quantity Needed per Device</t>
+  </si>
+  <si>
+    <t>32MB Flash Memory</t>
+  </si>
+  <si>
+    <t>MEM_001</t>
+  </si>
+  <si>
+    <t>256MB Flash Memory</t>
+  </si>
+  <si>
+    <t>MEM_002</t>
+  </si>
+  <si>
+    <t>1GB Flash Memory</t>
+  </si>
+  <si>
+    <t>MEM_003</t>
+  </si>
+  <si>
+    <t>ATMEGA 2560 Microcontroller</t>
+  </si>
+  <si>
+    <t>CON_001</t>
+  </si>
+  <si>
+    <t>PIC24FJ256GB610 Microcontroller</t>
+  </si>
+  <si>
+    <t>CON_002</t>
+  </si>
+  <si>
+    <t>AT32UC3A3256 Microcontroller</t>
+  </si>
+  <si>
+    <t>CON_003</t>
+  </si>
+  <si>
+    <t>ADXL343BCCZ Accelerometer</t>
+  </si>
+  <si>
+    <t>MOT_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3GD20H Gyroscope </t>
+  </si>
+  <si>
+    <t>MOT_002</t>
+  </si>
+  <si>
+    <t>Acc and Gyro Combo</t>
+  </si>
+  <si>
+    <t>MOT_003</t>
+  </si>
+  <si>
+    <t>RS PRO Piezo Pad</t>
+  </si>
+  <si>
+    <t>PRE_001</t>
+  </si>
+  <si>
+    <t>BM1383AGLV Pressure Sensor</t>
+  </si>
+  <si>
+    <t>PRE_002</t>
+  </si>
+  <si>
+    <t>Pieze and Pressure Combo</t>
+  </si>
+  <si>
+    <t>PRE_003</t>
+  </si>
+  <si>
+    <t>MAX30101 Heart Rate Sensor</t>
+  </si>
+  <si>
+    <t>HRT_001</t>
+  </si>
+  <si>
+    <t>BH1792GL Heart Rate Sensor</t>
+  </si>
+  <si>
+    <t>HRT_002</t>
+  </si>
+  <si>
+    <t>SGPC3 Air Quality Sensor</t>
+  </si>
+  <si>
+    <t>AIR_001</t>
+  </si>
+  <si>
+    <t>AS-MLV-P2 Air Quality Sensor</t>
+  </si>
+  <si>
+    <t>AIR_002</t>
+  </si>
+  <si>
+    <t>Rigid PCB</t>
+  </si>
+  <si>
+    <t>PCB_001</t>
+  </si>
+  <si>
+    <t>Flexi PCB</t>
+  </si>
+  <si>
+    <t>PCB_002</t>
+  </si>
+  <si>
+    <t>BGX13S Bluetooth Module</t>
+  </si>
+  <si>
+    <t>BLE_001</t>
+  </si>
+  <si>
+    <t>BlueNor_BT832 Bluetooth Module</t>
+  </si>
+  <si>
+    <t>BLE_002</t>
+  </si>
+  <si>
+    <t>ESP8266EX WiFi Module</t>
+  </si>
+  <si>
+    <t>WIFI_001</t>
+  </si>
+  <si>
+    <t>ACAG0301(Dual Band Antenna)</t>
+  </si>
+  <si>
+    <t>WANT_001</t>
+  </si>
+  <si>
+    <t>ACAG0201(Single Band Antenna)</t>
+  </si>
+  <si>
+    <t>WANT_002</t>
+  </si>
+  <si>
+    <t>Telit J-F2 (+ ACAG0301 1.5GHz Antenna)</t>
+  </si>
+  <si>
+    <t>GPS_001</t>
+  </si>
+  <si>
+    <t>Telit SL869 (+ ACAG0301 1.5GHz Antenna)</t>
+  </si>
+  <si>
+    <t>GPS_002</t>
+  </si>
+  <si>
+    <t>Quectel L80-M39 (GPS &amp; Integrated Antenna)</t>
+  </si>
+  <si>
+    <t>GPS_003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,14 +240,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -160,7 +278,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -172,7 +290,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -219,6 +337,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -254,6 +389,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -406,25 +558,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -441,13 +595,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>19.39</v>
+        <v>1.2033</v>
       </c>
       <c r="D2">
-        <v>4000</v>
+        <v>22.5</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -455,16 +609,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>21.39</v>
+        <v>2.15333</v>
       </c>
       <c r="D3">
-        <v>6000</v>
+        <v>22.5</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -472,16 +626,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>17.39</v>
+        <v>1.7344999999999999</v>
       </c>
       <c r="D4">
-        <v>8000</v>
+        <v>22.5</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -489,67 +643,67 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>20.18</v>
+        <v>7.6751399999999999</v>
       </c>
       <c r="D5">
-        <v>10000</v>
+        <v>307.2</v>
       </c>
       <c r="E5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>22.18</v>
-      </c>
-      <c r="D6">
-        <v>15000</v>
+        <v>2.8155000000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>172.8</v>
       </c>
       <c r="E6">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>24.18</v>
-      </c>
-      <c r="D7">
-        <v>8000</v>
+        <v>7.5825600000000009</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.4500000000000002</v>
       </c>
       <c r="E7">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>0.11</v>
-      </c>
-      <c r="D8">
-        <v>10000</v>
+        <v>1.2072000000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>15</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -557,16 +711,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>0.31</v>
-      </c>
-      <c r="D9">
-        <v>8000</v>
+        <v>1.2490299999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>9</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -574,22 +728,553 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10">
-        <v>0.21</v>
+        <v>2.4562300000000001</v>
       </c>
       <c r="D10">
-        <v>6000</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="D11">
+        <v>572.6</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>1.8662599999999998</v>
+      </c>
+      <c r="D12">
+        <v>6.25</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>2.1622599999999998</v>
+      </c>
+      <c r="D13">
+        <v>578.85</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>4.8464999999999998</v>
+      </c>
+      <c r="D14">
+        <v>28.6</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>4.1099600000000001</v>
+      </c>
+      <c r="D15">
+        <v>7.84</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16">
+        <v>4.4587599999999998</v>
+      </c>
+      <c r="D16">
+        <v>5.4</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>10.06</v>
+      </c>
+      <c r="D17">
+        <v>372.65</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="D18">
+        <v>5000</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>25.37</v>
+      </c>
+      <c r="D19">
+        <v>5000</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>6.19</v>
+      </c>
+      <c r="D20">
+        <v>81</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21">
+        <v>3.89</v>
+      </c>
+      <c r="D21">
+        <v>455</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22">
+        <v>1.22</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="D23">
+        <v>36</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>0.22</v>
+      </c>
+      <c r="D24">
+        <v>22</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25">
+        <v>7.1660000000000004</v>
+      </c>
+      <c r="D25">
+        <v>332</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26">
+        <v>14.148</v>
+      </c>
+      <c r="D26">
+        <v>487</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27">
+        <v>14.79</v>
+      </c>
+      <c r="D27">
+        <v>1651</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010002446F084470B3468887C48FC456BDE0" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a2186b1d035bb4c249b17abb53e72c2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="12e6bdaa-c140-42bc-8573-b4b2dcfaf07b" xmlns:ns3="7ceff3d1-26d0-4a19-9784-ffc192f0c3e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5d00ca550f340edf69a56c0ba3561b2" ns2:_="" ns3:_="">
+    <xsd:import namespace="12e6bdaa-c140-42bc-8573-b4b2dcfaf07b"/>
+    <xsd:import namespace="7ceff3d1-26d0-4a19-9784-ffc192f0c3e4"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="12e6bdaa-c140-42bc-8573-b4b2dcfaf07b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="14" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7ceff3d1-26d0-4a19-9784-ffc192f0c3e4" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9F51C09-4F5C-4C59-A9AB-EC6DE55A1AE5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{815843A1-5D2D-4E1E-A0EC-1A0B938D2C9A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="12e6bdaa-c140-42bc-8573-b4b2dcfaf07b"/>
+    <ds:schemaRef ds:uri="7ceff3d1-26d0-4a19-9784-ffc192f0c3e4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFCF39D-C9BE-44F6-A931-23243895FC97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Final update with all components accounted for
</commit_message>
<xml_diff>
--- a/GDBP/Device Permutations/components.xlsx
+++ b/GDBP/Device Permutations/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\Programming\Uni\trunk\GDBP\Device Permutations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1931ECB-6821-4C3A-9A96-FA626687C2FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1527DAFB-04DA-412A-9BFC-6B209884A561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Component Name</t>
   </si>
@@ -86,9 +86,6 @@
     <t>MOT_001</t>
   </si>
   <si>
-    <t xml:space="preserve">L3GD20H Gyroscope </t>
-  </si>
-  <si>
     <t>MOT_002</t>
   </si>
   <si>
@@ -198,23 +195,43 @@
   </si>
   <si>
     <t>GPS_003</t>
+  </si>
+  <si>
+    <t>L3GD20H Gyroscope </t>
+  </si>
+  <si>
+    <t>18650 Rechargeable Lithium Cell - 3.7 V 2500 mAh </t>
+  </si>
+  <si>
+    <t>BAT_001</t>
+  </si>
+  <si>
+    <t>Panasonic CR2032 DL2032 3V Lithium Coin Batteries</t>
+  </si>
+  <si>
+    <t>BAT_002</t>
+  </si>
+  <si>
+    <t>BAT_003</t>
+  </si>
+  <si>
+    <t>BAT_004</t>
+  </si>
+  <si>
+    <t>CGAS007 Energizer Single Cell 3.7 V Lithium Ion 1 Ah</t>
+  </si>
+  <si>
+    <t>CA5L Energizer Single Cell 3.7 V Lithium Ion 980 mAh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,10 +257,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,466 +592,535 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1.2033</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>22.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2.15333</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>22.5</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1.7344999999999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>22.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>7.6751399999999999</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>307.2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>2.8155000000000001</v>
       </c>
       <c r="D6" s="1">
         <v>172.8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
-        <v>7.5825600000000009</v>
+      <c r="C7" s="1">
+        <v>7.58256</v>
       </c>
       <c r="D7" s="1">
         <v>2.4500000000000002</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>1.2072000000000001</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>15</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="1">
+        <v>1.2490300000000001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
-        <v>1.2490299999999999</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.4562300000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>572.6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.86626</v>
+      </c>
+      <c r="D12" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.1622599999999998</v>
+      </c>
+      <c r="D13" s="1">
+        <v>578.85</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4.8464999999999998</v>
+      </c>
+      <c r="D14" s="1">
+        <v>28.6</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4.1099600000000001</v>
+      </c>
+      <c r="D15" s="1">
+        <v>7.84</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4.4587599999999998</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10.06</v>
+      </c>
+      <c r="D17" s="1">
+        <v>372.65</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1">
+        <v>25.37</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6.19</v>
+      </c>
+      <c r="D20" s="1">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.89</v>
+      </c>
+      <c r="D21" s="1">
+        <v>455</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="D22" s="1">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="D23" s="1">
+        <v>36</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="D24" s="1">
+        <v>22</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="1">
+        <v>7.1660000000000004</v>
+      </c>
+      <c r="D25" s="1">
+        <v>332</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="1">
+        <v>14.148</v>
+      </c>
+      <c r="D26" s="1">
+        <v>487</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="1">
+        <v>14.79</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1651</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>131250</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1280</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="1">
         <v>9</v>
       </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10">
-        <v>2.4562300000000001</v>
-      </c>
-      <c r="D10">
-        <v>24</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="D11">
-        <v>572.6</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
-        <v>1.8662599999999998</v>
-      </c>
-      <c r="D12">
-        <v>6.25</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13">
-        <v>2.1622599999999998</v>
-      </c>
-      <c r="D13">
-        <v>578.85</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14">
-        <v>4.8464999999999998</v>
-      </c>
-      <c r="D14">
-        <v>28.6</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15">
-        <v>4.1099600000000001</v>
-      </c>
-      <c r="D15">
-        <v>7.84</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16">
-        <v>4.4587599999999998</v>
-      </c>
-      <c r="D16">
-        <v>5.4</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17">
-        <v>10.06</v>
-      </c>
-      <c r="D17">
-        <v>372.65</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18">
-        <v>8.4600000000000009</v>
-      </c>
-      <c r="D18">
-        <v>5000</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19">
-        <v>25.37</v>
-      </c>
-      <c r="D19">
-        <v>5000</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20">
-        <v>6.19</v>
-      </c>
-      <c r="D20">
-        <v>81</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21">
-        <v>3.89</v>
-      </c>
-      <c r="D21">
-        <v>455</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22">
-        <v>1.22</v>
-      </c>
-      <c r="D22">
-        <v>25</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23">
-        <v>0.77100000000000002</v>
-      </c>
-      <c r="D23">
-        <v>36</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24">
-        <v>0.22</v>
-      </c>
-      <c r="D24">
-        <v>22</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25">
-        <v>7.1660000000000004</v>
-      </c>
-      <c r="D25">
-        <v>332</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26">
-        <v>14.148</v>
-      </c>
-      <c r="D26">
-        <v>487</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27">
-        <v>14.79</v>
-      </c>
-      <c r="D27">
-        <v>1651</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
+      <c r="D30" s="1">
+        <v>13320</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="1">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1">
+        <v>11520</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Final(!) update with all components accounted for (now also doing enclosures you see)
</commit_message>
<xml_diff>
--- a/GDBP/Device Permutations/components.xlsx
+++ b/GDBP/Device Permutations/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\Programming\Uni\trunk\GDBP\Device Permutations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1527DAFB-04DA-412A-9BFC-6B209884A561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248E7DC4-B821-4AA1-8F5A-A0931365D6B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Component Name</t>
   </si>
@@ -218,10 +218,28 @@
     <t>BAT_004</t>
   </si>
   <si>
-    <t>CGAS007 Energizer Single Cell 3.7 V Lithium Ion 1 Ah</t>
-  </si>
-  <si>
-    <t>CA5L Energizer Single Cell 3.7 V Lithium Ion 980 mAh</t>
+    <t>CGAS007 Energizer Single Cell, 3.7 V, Lithium Ion, 1 Ah</t>
+  </si>
+  <si>
+    <t>CA5L Energizer Single Cell, 3.7 V, Lithium Ion, 980 mAh</t>
+  </si>
+  <si>
+    <t>2x Clip on Pod Enclosures</t>
+  </si>
+  <si>
+    <t>ENC_001</t>
+  </si>
+  <si>
+    <t>2x Insole with Removable Pod Enclosure</t>
+  </si>
+  <si>
+    <t>ENC_002</t>
+  </si>
+  <si>
+    <t>2x Insole with Attachable Pod Enclosure</t>
+  </si>
+  <si>
+    <t>ENC_003</t>
   </si>
 </sst>
 </file>
@@ -576,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,6 +1136,57 @@
         <v>2</v>
       </c>
     </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2.8544</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="1">
+        <v>8.0434000000000001</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="1">
+        <v>7.5095999999999998</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1125,12 +1194,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1325,15 +1391,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9F51C09-4F5C-4C59-A9AB-EC6DE55A1AE5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFCF39D-C9BE-44F6-A931-23243895FC97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1358,10 +1428,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFCF39D-C9BE-44F6-A931-23243895FC97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9F51C09-4F5C-4C59-A9AB-EC6DE55A1AE5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated logic so script is suited for dynamic changes to the input (i.e. no code change needed to add more component types)
</commit_message>
<xml_diff>
--- a/GDBP/Device Permutations/components.xlsx
+++ b/GDBP/Device Permutations/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\Programming\Uni\trunk\GDBP\Device Permutations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248E7DC4-B821-4AA1-8F5A-A0931365D6B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2140F465-D28C-4A39-925D-F30E5022EF39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,12 +218,6 @@
     <t>BAT_004</t>
   </si>
   <si>
-    <t>CGAS007 Energizer Single Cell, 3.7 V, Lithium Ion, 1 Ah</t>
-  </si>
-  <si>
-    <t>CA5L Energizer Single Cell, 3.7 V, Lithium Ion, 980 mAh</t>
-  </si>
-  <si>
     <t>2x Clip on Pod Enclosures</t>
   </si>
   <si>
@@ -240,6 +234,12 @@
   </si>
   <si>
     <t>ENC_003</t>
+  </si>
+  <si>
+    <t>CGAS007 Energizer Single Cell 3.7 V Lithium Ion 1 Ah</t>
+  </si>
+  <si>
+    <t>CA5L Energizer Single Cell 3.7 V Lithium Ion 980 mAh</t>
   </si>
 </sst>
 </file>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>61</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>62</v>
@@ -1138,10 +1138,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32" s="1">
         <v>2.8544</v>
@@ -1155,10 +1155,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C33" s="1">
         <v>8.0434000000000001</v>
@@ -1172,10 +1172,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" s="1">
         <v>7.5095999999999998</v>
@@ -1194,9 +1194,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1391,19 +1394,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFCF39D-C9BE-44F6-A931-23243895FC97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9F51C09-4F5C-4C59-A9AB-EC6DE55A1AE5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1428,9 +1427,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9F51C09-4F5C-4C59-A9AB-EC6DE55A1AE5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFCF39D-C9BE-44F6-A931-23243895FC97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated component input file given additional enclosure types.
More comments for the script in case I die
</commit_message>
<xml_diff>
--- a/GDBP/Device Permutations/components.xlsx
+++ b/GDBP/Device Permutations/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\Programming\Uni\trunk\GDBP\Device Permutations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2140F465-D28C-4A39-925D-F30E5022EF39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D81799C-A9FD-475E-A479-0D788AECDEC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Component Name</t>
   </si>
@@ -224,15 +224,9 @@
     <t>ENC_001</t>
   </si>
   <si>
-    <t>2x Insole with Removable Pod Enclosure</t>
-  </si>
-  <si>
     <t>ENC_002</t>
   </si>
   <si>
-    <t>2x Insole with Attachable Pod Enclosure</t>
-  </si>
-  <si>
     <t>ENC_003</t>
   </si>
   <si>
@@ -240,6 +234,24 @@
   </si>
   <si>
     <t>CA5L Energizer Single Cell 3.7 V Lithium Ion 980 mAh</t>
+  </si>
+  <si>
+    <t>2x Manufactured Insole with Removable Pod Enclosure</t>
+  </si>
+  <si>
+    <t>2x Manufactured Insole with Attachable Pod Enclosure</t>
+  </si>
+  <si>
+    <t>2x Purchased Insole with Removable Pod Enclosure</t>
+  </si>
+  <si>
+    <t>ENC_004</t>
+  </si>
+  <si>
+    <t>2x Purchased Insole with Attachable Pod Enclosure</t>
+  </si>
+  <si>
+    <t>ENC_005</t>
   </si>
 </sst>
 </file>
@@ -594,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,7 +1116,7 @@
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>61</v>
@@ -1121,7 +1133,7 @@
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>62</v>
@@ -1153,12 +1165,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C33" s="1">
         <v>8.0434000000000001</v>
@@ -1170,12 +1182,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="1">
         <v>7.5095999999999998</v>
@@ -1184,6 +1196,40 @@
         <v>0</v>
       </c>
       <c r="E34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3.9658000000000002</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4.3433999999999999</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1194,12 +1240,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1394,15 +1437,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9F51C09-4F5C-4C59-A9AB-EC6DE55A1AE5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFCF39D-C9BE-44F6-A931-23243895FC97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1427,10 +1474,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFCF39D-C9BE-44F6-A931-23243895FC97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9F51C09-4F5C-4C59-A9AB-EC6DE55A1AE5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Started gait ui project
</commit_message>
<xml_diff>
--- a/GDBP/Device Permutations/components.xlsx
+++ b/GDBP/Device Permutations/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blaze\Desktop\Programming\Uni\trunk\GDBP\Device Permutations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D81799C-A9FD-475E-A479-0D788AECDEC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A1E48D-8EF0-4979-8D43-5EEBB1FD5083}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1207,7 +1207,7 @@
         <v>72</v>
       </c>
       <c r="C35" s="1">
-        <v>3.9658000000000002</v>
+        <v>2.9157999999999999</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
@@ -1224,7 +1224,7 @@
         <v>74</v>
       </c>
       <c r="C36" s="1">
-        <v>4.3433999999999999</v>
+        <v>3.2934000000000001</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
@@ -1246,6 +1246,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010002446F084470B3468887C48FC456BDE0" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a2186b1d035bb4c249b17abb53e72c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="12e6bdaa-c140-42bc-8573-b4b2dcfaf07b" xmlns:ns3="7ceff3d1-26d0-4a19-9784-ffc192f0c3e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5d00ca550f340edf69a56c0ba3561b2" ns2:_="" ns3:_="">
     <xsd:import namespace="12e6bdaa-c140-42bc-8573-b4b2dcfaf07b"/>
@@ -1436,15 +1445,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CFCF39D-C9BE-44F6-A931-23243895FC97}">
   <ds:schemaRefs>
@@ -1455,6 +1455,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9F51C09-4F5C-4C59-A9AB-EC6DE55A1AE5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{815843A1-5D2D-4E1E-A0EC-1A0B938D2C9A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1471,12 +1479,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9F51C09-4F5C-4C59-A9AB-EC6DE55A1AE5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>